<commit_message>
Digikey P/Ns to BOM, MPNs to some non-obvious sch components
</commit_message>
<xml_diff>
--- a/meng-spad-quenching/acq-rev1-bom.xlsx
+++ b/meng-spad-quenching/acq-rev1-bom.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Eagle-Public\meng-spad-quenching\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="aqc_rev1_bom" localSheetId="0">Sheet1!$A$1:$G$42</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="187">
   <si>
     <t>Part</t>
   </si>
@@ -59,33 +54,18 @@
     <t>100n</t>
   </si>
   <si>
-    <t>C-EUC0603</t>
-  </si>
-  <si>
     <t>C0603</t>
   </si>
   <si>
     <t>10n</t>
   </si>
   <si>
-    <t>C-EUC0402</t>
-  </si>
-  <si>
     <t>C0402</t>
   </si>
   <si>
     <t>C9</t>
   </si>
   <si>
-    <t>33u,</t>
-  </si>
-  <si>
-    <t>25V</t>
-  </si>
-  <si>
-    <t>CPOL-EUCT7343</t>
-  </si>
-  <si>
     <t>C23</t>
   </si>
   <si>
@@ -95,9 +75,6 @@
     <t>10u</t>
   </si>
   <si>
-    <t>C-EUC1206</t>
-  </si>
-  <si>
     <t>C1206</t>
   </si>
   <si>
@@ -107,9 +84,6 @@
     <t>SD101BW-TP</t>
   </si>
   <si>
-    <t>DIODE-SOD123</t>
-  </si>
-  <si>
     <t>SOD123</t>
   </si>
   <si>
@@ -119,15 +93,9 @@
     <t>ADCMP582</t>
   </si>
   <si>
-    <t>QFN50P300X300X80-16N</t>
-  </si>
-  <si>
     <t>OPA342</t>
   </si>
   <si>
-    <t>OPA333DBV</t>
-  </si>
-  <si>
     <t>SOT23-5</t>
   </si>
   <si>
@@ -137,9 +105,6 @@
     <t>NC7SV74K8X</t>
   </si>
   <si>
-    <t>US8_3.1MM_JDEC_MO-187</t>
-  </si>
-  <si>
     <t>IC5</t>
   </si>
   <si>
@@ -164,21 +129,12 @@
     <t>DS1100LU-20+</t>
   </si>
   <si>
-    <t>DS1100L</t>
-  </si>
-  <si>
     <t>IC8</t>
   </si>
   <si>
     <t>LT3032-5</t>
   </si>
   <si>
-    <t>LT3032</t>
-  </si>
-  <si>
-    <t>DFN14-4X3DE</t>
-  </si>
-  <si>
     <t>IC9</t>
   </si>
   <si>
@@ -191,42 +147,24 @@
     <t>VIN_LOGIC</t>
   </si>
   <si>
-    <t>CONN_MOLEX_3PIN_MINI-FIT_JR</t>
-  </si>
-  <si>
     <t>LEDCHIP-LED0805</t>
   </si>
   <si>
-    <t>CHIP-LED0805</t>
-  </si>
-  <si>
-    <t>led</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
     <t>BSS806N</t>
   </si>
   <si>
-    <t>SOT23R_INFINEON</t>
-  </si>
-  <si>
     <t>MMBTH81</t>
   </si>
   <si>
-    <t>MMBTH81LT1SMD</t>
-  </si>
-  <si>
     <t>SOT23-BEC</t>
   </si>
   <si>
     <t>DNP</t>
   </si>
   <si>
-    <t>R-EU_R0603</t>
-  </si>
-  <si>
     <t>R0603</t>
   </si>
   <si>
@@ -239,9 +177,6 @@
     <t>150R</t>
   </si>
   <si>
-    <t>R-EU_R0402</t>
-  </si>
-  <si>
     <t>R0402</t>
   </si>
   <si>
@@ -266,18 +201,12 @@
     <t>100R</t>
   </si>
   <si>
-    <t>R-EU_R0805</t>
-  </si>
-  <si>
     <t>R0805</t>
   </si>
   <si>
     <t>3269W-1-102LF</t>
   </si>
   <si>
-    <t>BOURNS_3269WX</t>
-  </si>
-  <si>
     <t>3269W</t>
   </si>
   <si>
@@ -287,24 +216,12 @@
     <t>MMBTH10</t>
   </si>
   <si>
-    <t>MMBTH10LT1-NPN-SOT23-BEC</t>
-  </si>
-  <si>
-    <t>KEYSTONE_5000</t>
-  </si>
-  <si>
-    <t>KEYSTONE_5000_MINIATURE</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
     <t>SN65EPT21DGK</t>
   </si>
   <si>
-    <t>SOP65P490X110-8N</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -317,15 +234,6 @@
     <t>TPS78233DDCT</t>
   </si>
   <si>
-    <t>SOT95P280X110-5N</t>
-  </si>
-  <si>
-    <t>SMA-142-0711-871/876</t>
-  </si>
-  <si>
-    <t>J502-ND-142-0711-871/876</t>
-  </si>
-  <si>
     <t>aqc-rev1 BOM</t>
   </si>
   <si>
@@ -368,9 +276,6 @@
     <t>TP2, TP10, TP11, TP12. TP13</t>
   </si>
   <si>
-    <t>Colored TP VREF</t>
-  </si>
-  <si>
     <t>Black TP GND</t>
   </si>
   <si>
@@ -401,9 +306,6 @@
     <t>R36, R37</t>
   </si>
   <si>
-    <t>470R (LED?)</t>
-  </si>
-  <si>
     <t>R1, R21, R29, R30, R31, R32, R33, R34, R35, R38, R39, R40, R41, R42, R43</t>
   </si>
   <si>
@@ -423,13 +325,292 @@
   </si>
   <si>
     <t>C36, C38, C41, C44, C46, C47</t>
+  </si>
+  <si>
+    <t>SD101BWTPMSCT-ND</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 50V 15MA SOD123</t>
+  </si>
+  <si>
+    <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>ADCMP582BCPZ-WP</t>
+  </si>
+  <si>
+    <t>IC COMPARATOR PECL UFAST 16LFCSP</t>
+  </si>
+  <si>
+    <t>Note: Cost is with MIT negotiated price.</t>
+  </si>
+  <si>
+    <t>296-41474-1-ND</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 1MHZ RRO SOT23-5</t>
+  </si>
+  <si>
+    <t>NC7SV74K8XCT-ND</t>
+  </si>
+  <si>
+    <t>IC D-TYPE POS TRG SNGL US8</t>
+  </si>
+  <si>
+    <t>NC7WZ16P6XCT-ND</t>
+  </si>
+  <si>
+    <t>IC BUFFER DL UHS N-INV SC70-6</t>
+  </si>
+  <si>
+    <t>LT1711CMS8#PBF-ND</t>
+  </si>
+  <si>
+    <t>IC COMP R-RINOUT SINGLE 8-MSOP</t>
+  </si>
+  <si>
+    <t>DS1100LU-20+-ND</t>
+  </si>
+  <si>
+    <t>IC DELAY LINE 5TAP 20NS 8UMAX</t>
+  </si>
+  <si>
+    <t>LT3032EDE-5#PBF-ND</t>
+  </si>
+  <si>
+    <t>IC REG LDO +-5V 0.15A 14DFN</t>
+  </si>
+  <si>
+    <t>LT3032EDE-15#PBF-ND</t>
+  </si>
+  <si>
+    <t>IC REG LDO +-15V 0.15A 14DFN</t>
+  </si>
+  <si>
+    <t>BSS806N H6327CT-ND</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 20V 2.3A SOT23</t>
+  </si>
+  <si>
+    <t>MMBTH81CT-ND</t>
+  </si>
+  <si>
+    <t>TRANSISTOR RF PNP SOT-23</t>
+  </si>
+  <si>
+    <t>MMBTH10-4LT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>TRANS VHF/UHF NPN 25V SOT-23</t>
+  </si>
+  <si>
+    <t>IC XLATR DIFF PECL/LVDS 8VSSOP</t>
+  </si>
+  <si>
+    <t>296-27264-5-ND</t>
+  </si>
+  <si>
+    <t>296-24086-5-ND</t>
+  </si>
+  <si>
+    <t>BUFFER DUAL LVPECL 3.3V 8VSSOP</t>
+  </si>
+  <si>
+    <t>296-24120-1-ND</t>
+  </si>
+  <si>
+    <t>IC REG LDO 3.3V 0.15A 5SOT</t>
+  </si>
+  <si>
+    <t>36-5001-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC MINI .040"D BLACK</t>
+  </si>
+  <si>
+    <t>TEST POINT PC MINI .040"D WHITE</t>
+  </si>
+  <si>
+    <t>36-5002-ND</t>
+  </si>
+  <si>
+    <t>White TP VREF</t>
+  </si>
+  <si>
+    <t>3269W-1-102LF-ND</t>
+  </si>
+  <si>
+    <t>TRIMMER 1K OHM 0.25W SMD</t>
+  </si>
+  <si>
+    <t>563-1022-1-ND</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE DIP SPDT 100MA 6V</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD49R9CT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 49.9 OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD1K00CT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>311-1.43KHRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 1.43K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT470RCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 470 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>16LFCSP</t>
+  </si>
+  <si>
+    <t>US8</t>
+  </si>
+  <si>
+    <t>C7343</t>
+  </si>
+  <si>
+    <t>14DFN</t>
+  </si>
+  <si>
+    <t>LED0805</t>
+  </si>
+  <si>
+    <t>SOT23R</t>
+  </si>
+  <si>
+    <t>8VSSOP</t>
+  </si>
+  <si>
+    <t>5SOT</t>
+  </si>
+  <si>
+    <t>SMA-SMT</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>311-0.0GRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
+    <t>P150LCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 150 OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>P100LCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 1% 1/10W 0402</t>
+  </si>
+  <si>
+    <t>732-4986-1-ND</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>311-150CRCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 150 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>DNP, Buy Extra 0R Jumpers</t>
+  </si>
+  <si>
+    <t>490-1312-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 25V X7R 0402</t>
+  </si>
+  <si>
+    <t>1276-1132-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>490-1524-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>490-10698-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0402</t>
+  </si>
+  <si>
+    <t>490-6518-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V X7R 1206</t>
+  </si>
+  <si>
+    <t>PCF1453CT-ND</t>
+  </si>
+  <si>
+    <t>CAP FILM 1000PF 2% 16VDC 0603</t>
+  </si>
+  <si>
+    <t>33u</t>
+  </si>
+  <si>
+    <t>P16819-1-ND</t>
+  </si>
+  <si>
+    <t>CAP ALUM POLY 33UF 20% 25V SMD</t>
+  </si>
+  <si>
+    <t>WM7251-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER 3POS SNGL VERT GOLD</t>
+  </si>
+  <si>
+    <t>WM5534-ND</t>
+  </si>
+  <si>
+    <t>CONN SMA JACK 50 OHM EDGE MNT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +620,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -463,14 +651,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,7 +725,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,7 +760,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -745,7 +937,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,27 +945,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -784,688 +982,1087 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>97</v>
+        <v>66</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>98</v>
+        <v>67</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>173</v>
+      </c>
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.09</v>
       </c>
       <c r="H4">
         <v>6</v>
       </c>
+      <c r="I4" s="2">
+        <f>G4*H4</f>
+        <v>0.54</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>169</v>
+      </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.09</v>
       </c>
       <c r="H5">
         <v>14</v>
       </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I42" si="0">G5*H5</f>
+        <v>1.26</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>171</v>
+      </c>
+      <c r="F6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.09</v>
       </c>
       <c r="H6">
         <v>8</v>
       </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.09</v>
       </c>
       <c r="H7">
         <v>11</v>
       </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>182</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.45</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.45</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>179</v>
+      </c>
+      <c r="F9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.38</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>177</v>
+      </c>
+      <c r="F10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.22</v>
       </c>
       <c r="H10">
         <v>6</v>
       </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.32</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.3</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>99</v>
+      </c>
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="2">
+        <v>15.89</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>15.89</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
         <v>101</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
+      <c r="G13" s="2">
+        <v>0.97</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.94</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.51</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>106</v>
+      </c>
+      <c r="F15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.34</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>108</v>
+      </c>
+      <c r="F16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4.4000000000000004</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>110</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="2">
+        <v>5.14</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>5.14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>112</v>
+      </c>
+      <c r="F18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="2">
+        <v>4.7</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>114</v>
+      </c>
+      <c r="F19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="2">
+        <v>4.7</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>184</v>
+      </c>
+      <c r="F20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.2</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>163</v>
+      </c>
+      <c r="F21" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.28999999999999998</v>
       </c>
       <c r="H21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>116</v>
+      </c>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.3</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>118</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.19</v>
       </c>
       <c r="H23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1400000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>167</v>
+      </c>
+      <c r="F24" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
       </c>
       <c r="H24">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>137</v>
+      </c>
+      <c r="F25" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.09</v>
       </c>
       <c r="H25">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.80999999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>139</v>
+      </c>
+      <c r="F26" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.09</v>
       </c>
       <c r="H26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>159</v>
+      </c>
+      <c r="F27" t="s">
+        <v>158</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.09</v>
       </c>
       <c r="H27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>141</v>
+      </c>
+      <c r="F28" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.09</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
+        <v>143</v>
+      </c>
+      <c r="F29" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.09</v>
       </c>
       <c r="H29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
+        <v>155</v>
+      </c>
+      <c r="F30" t="s">
+        <v>154</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.09</v>
       </c>
       <c r="H30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>59</v>
+        <v>157</v>
+      </c>
+      <c r="F31" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.09</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
+        <v>161</v>
+      </c>
+      <c r="F32" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.09</v>
       </c>
       <c r="H32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>165</v>
+      </c>
+      <c r="F33" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.09</v>
       </c>
       <c r="H33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>133</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" s="2">
+        <v>4.1100000000000003</v>
       </c>
       <c r="H34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="2">
+        <f t="shared" si="0"/>
+        <v>16.440000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>135</v>
+      </c>
+      <c r="F35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.73</v>
       </c>
       <c r="H35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>120</v>
+      </c>
+      <c r="F36" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.23</v>
       </c>
       <c r="H36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="2">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>129</v>
+      </c>
+      <c r="F37" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.32</v>
       </c>
       <c r="H37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>128</v>
+      </c>
+      <c r="F38" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.32</v>
       </c>
       <c r="H38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>121</v>
+      </c>
+      <c r="F39" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" s="2">
+        <v>3.4</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>124</v>
+      </c>
+      <c r="F40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3.4</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>126</v>
+      </c>
+      <c r="F41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.74</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>186</v>
+      </c>
+      <c r="F42" t="s">
+        <v>185</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2.84</v>
       </c>
       <c r="H42">
         <v>6</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="0"/>
+        <v>17.04</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I45" s="2">
+        <f>SUM(I4:I42)</f>
+        <v>97.380000000000024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added BOM# column to BOM
</commit_message>
<xml_diff>
--- a/meng-spad-quenching/acq-rev1-bom.xlsx
+++ b/meng-spad-quenching/acq-rev1-bom.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Eagle-Public\meng-spad-quenching\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="aqc_rev1_bom" localSheetId="0">Sheet1!$A$1:$G$42</definedName>
+    <definedName name="aqc_rev1_bom" localSheetId="0">Sheet1!$B$1:$H$42</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="196">
   <si>
     <t>Part</t>
   </si>
@@ -342,9 +347,6 @@
     <t>IC COMPARATOR PECL UFAST 16LFCSP</t>
   </si>
   <si>
-    <t>Note: Cost is with MIT negotiated price.</t>
-  </si>
-  <si>
     <t>296-41474-1-ND</t>
   </si>
   <si>
@@ -601,6 +603,36 @@
   </si>
   <si>
     <t>CONN SMA JACK 50 OHM EDGE MNT</t>
+  </si>
+  <si>
+    <t>25V</t>
+  </si>
+  <si>
+    <t>50V</t>
+  </si>
+  <si>
+    <t>16V</t>
+  </si>
+  <si>
+    <t>20V</t>
+  </si>
+  <si>
+    <t>1/8W</t>
+  </si>
+  <si>
+    <t>1/10W</t>
+  </si>
+  <si>
+    <t>0.25W</t>
+  </si>
+  <si>
+    <t>6V</t>
+  </si>
+  <si>
+    <t>Note: Cost is with MIT negotiated price, bulk discount not included.</t>
+  </si>
+  <si>
+    <t>BOM #</t>
   </si>
 </sst>
 </file>
@@ -610,7 +642,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,16 +665,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -650,18 +695,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -937,7 +1000,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -945,1123 +1008,1344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>173</v>
       </c>
       <c r="F4" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.09</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>6</v>
       </c>
-      <c r="I4" s="2">
-        <f>G4*H4</f>
+      <c r="J4" s="4">
+        <f>H4*I4</f>
         <v>0.54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>A4+1</f>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>169</v>
       </c>
       <c r="F5" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.09</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>14</v>
       </c>
-      <c r="I5" s="2">
-        <f t="shared" ref="I5:I42" si="0">G5*H5</f>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J42" si="0">H5*I5</f>
         <v>1.26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ref="A6:A42" si="1">A5+1</f>
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" t="s">
         <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>171</v>
       </c>
       <c r="F6" t="s">
         <v>170</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="2">
         <v>0.09</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>8</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="4">
         <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>90</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>175</v>
       </c>
       <c r="F7" t="s">
         <v>174</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="2">
         <v>0.09</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>11</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="4">
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>180</v>
+      <c r="C8" t="s">
+        <v>179</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="E8" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="F8" t="s">
         <v>181</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="2">
         <v>1.45</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="4">
         <f t="shared" si="0"/>
         <v>1.45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" t="s">
         <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>179</v>
       </c>
       <c r="F9" t="s">
         <v>178</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" s="2">
         <v>0.38</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="4">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>94</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
+        <v>186</v>
+      </c>
+      <c r="E10" t="s">
         <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>177</v>
       </c>
       <c r="F10" t="s">
         <v>176</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" t="s">
+        <v>175</v>
+      </c>
+      <c r="H10" s="2">
         <v>0.22</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>6</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="4">
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>96</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>95</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>0.3</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="4">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
-        <v>144</v>
-      </c>
       <c r="E12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" t="s">
         <v>99</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>15.89</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="4">
         <f t="shared" si="0"/>
         <v>15.89</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>72</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>102</v>
       </c>
       <c r="F13" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="2">
         <v>0.97</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="4">
         <f t="shared" si="0"/>
         <v>1.94</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>145</v>
-      </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="F14" t="s">
         <v>103</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="2">
         <v>0.51</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>1</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="4">
         <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>106</v>
       </c>
       <c r="F15" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.34</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="4">
         <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>108</v>
       </c>
       <c r="F16" t="s">
         <v>107</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>1</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="4">
         <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>110</v>
       </c>
       <c r="F17" t="s">
         <v>109</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="2">
         <v>5.14</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>1</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="4">
         <f t="shared" si="0"/>
         <v>5.14</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
-        <v>147</v>
-      </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="2">
         <v>4.7</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="4">
         <f t="shared" si="0"/>
         <v>4.7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>32</v>
       </c>
-      <c r="D19" t="s">
-        <v>147</v>
-      </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
         <v>113</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="2">
         <v>4.7</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>1</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="4">
         <f t="shared" si="0"/>
         <v>4.7</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" t="s">
-        <v>153</v>
-      </c>
       <c r="E20" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="F20" t="s">
         <v>183</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" t="s">
+        <v>182</v>
+      </c>
+      <c r="H20" s="2">
         <v>1.2</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>1</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="4">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="D21" t="s">
-        <v>148</v>
-      </c>
       <c r="E21" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F21" t="s">
         <v>162</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" t="s">
+        <v>161</v>
+      </c>
+      <c r="H21" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="4">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="F22" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="2">
         <v>0.3</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>1</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="4">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>39</v>
-      </c>
-      <c r="E23" t="s">
-        <v>118</v>
       </c>
       <c r="F23" t="s">
         <v>117</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="2">
         <v>0.19</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>6</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="4">
         <f t="shared" si="0"/>
         <v>1.1400000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>40</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>41</v>
-      </c>
-      <c r="E24" t="s">
-        <v>167</v>
       </c>
       <c r="F24" t="s">
         <v>166</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" s="2">
         <v>0</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>15</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>A23+1</f>
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>42</v>
       </c>
       <c r="D25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" t="s">
         <v>41</v>
-      </c>
-      <c r="E25" t="s">
-        <v>137</v>
       </c>
       <c r="F25" t="s">
         <v>136</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="2">
         <v>0.09</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>9</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="4">
         <f t="shared" si="0"/>
         <v>0.80999999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
         <v>82</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>43</v>
       </c>
       <c r="D26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" t="s">
         <v>41</v>
-      </c>
-      <c r="E26" t="s">
-        <v>139</v>
       </c>
       <c r="F26" t="s">
         <v>138</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="2">
         <v>0.09</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>5</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="4">
         <f t="shared" si="0"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>81</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" t="s">
         <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>159</v>
       </c>
       <c r="F27" t="s">
         <v>158</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="2">
         <v>0.09</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>2</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="4">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>47</v>
       </c>
       <c r="D28" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" t="s">
         <v>41</v>
-      </c>
-      <c r="E28" t="s">
-        <v>141</v>
       </c>
       <c r="F28" t="s">
         <v>140</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="2">
         <v>0.09</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>1</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="4">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>48</v>
       </c>
       <c r="D29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" t="s">
         <v>41</v>
-      </c>
-      <c r="E29" t="s">
-        <v>143</v>
       </c>
       <c r="F29" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" s="2">
         <v>0.09</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>4</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="4">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
         <v>85</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>49</v>
       </c>
       <c r="D30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" t="s">
         <v>41</v>
-      </c>
-      <c r="E30" t="s">
-        <v>155</v>
       </c>
       <c r="F30" t="s">
         <v>154</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" t="s">
+        <v>153</v>
+      </c>
+      <c r="H30" s="2">
         <v>0.09</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>2</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="4">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>51</v>
       </c>
       <c r="D31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" t="s">
         <v>41</v>
-      </c>
-      <c r="E31" t="s">
-        <v>157</v>
       </c>
       <c r="F31" t="s">
         <v>156</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" t="s">
+        <v>155</v>
+      </c>
+      <c r="H31" s="2">
         <v>0.09</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>1</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="4">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
         <v>84</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>52</v>
       </c>
       <c r="D32" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" t="s">
         <v>45</v>
-      </c>
-      <c r="E32" t="s">
-        <v>161</v>
       </c>
       <c r="F32" t="s">
         <v>160</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" t="s">
+        <v>159</v>
+      </c>
+      <c r="H32" s="2">
         <v>0.09</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>2</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="4">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
         <v>87</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>44</v>
       </c>
       <c r="D33" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" t="s">
         <v>53</v>
-      </c>
-      <c r="E33" t="s">
-        <v>165</v>
       </c>
       <c r="F33" t="s">
         <v>164</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" t="s">
+        <v>163</v>
+      </c>
+      <c r="H33" s="2">
         <v>0.09</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="4">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>54</v>
       </c>
       <c r="D34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E34" t="s">
         <v>55</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
       </c>
       <c r="F34" t="s">
         <v>132</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="2">
         <v>4.1100000000000003</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>4</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="4">
         <f t="shared" si="0"/>
         <v>16.440000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
         <v>74</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>56</v>
       </c>
       <c r="D35" t="s">
+        <v>193</v>
+      </c>
+      <c r="E35" t="s">
         <v>56</v>
-      </c>
-      <c r="E35" t="s">
-        <v>135</v>
       </c>
       <c r="F35" t="s">
         <v>134</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="2">
         <v>0.73</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>3</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="4">
         <f t="shared" si="0"/>
         <v>2.19</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
         <v>75</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>57</v>
       </c>
       <c r="D36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" t="s">
         <v>39</v>
-      </c>
-      <c r="E36" t="s">
-        <v>120</v>
       </c>
       <c r="F36" t="s">
         <v>119</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" t="s">
+        <v>118</v>
+      </c>
+      <c r="H36" s="2">
         <v>0.23</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>7</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="4">
         <f t="shared" si="0"/>
         <v>1.61</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
         <v>77</v>
       </c>
-      <c r="B37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" t="s">
-        <v>153</v>
+      <c r="C37" t="s">
+        <v>130</v>
       </c>
       <c r="E37" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" t="s">
         <v>129</v>
       </c>
-      <c r="F37" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="2">
+      <c r="H37" s="2">
         <v>0.32</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>5</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="4">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
         <v>76</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>78</v>
       </c>
-      <c r="D38" t="s">
-        <v>153</v>
-      </c>
       <c r="E38" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="F38" t="s">
         <v>127</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" t="s">
+        <v>126</v>
+      </c>
+      <c r="H38" s="2">
         <v>0.32</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>2</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="4">
         <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>59</v>
       </c>
-      <c r="D39" t="s">
-        <v>150</v>
-      </c>
       <c r="E39" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" t="s">
         <v>121</v>
       </c>
-      <c r="F39" t="s">
-        <v>122</v>
-      </c>
-      <c r="G39" s="2">
+      <c r="H39" s="2">
         <v>3.4</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>1</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="4">
         <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
         <v>60</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>61</v>
       </c>
-      <c r="D40" t="s">
-        <v>150</v>
-      </c>
       <c r="E40" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="F40" t="s">
         <v>123</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" t="s">
+        <v>122</v>
+      </c>
+      <c r="H40" s="2">
         <v>3.4</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>1</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="4">
         <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B41" t="s">
         <v>62</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>63</v>
       </c>
-      <c r="D41" t="s">
-        <v>151</v>
-      </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="F41" t="s">
         <v>125</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" s="2">
         <v>0.74</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>1</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="4">
         <f t="shared" si="0"/>
         <v>0.74</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>79</v>
       </c>
-      <c r="D42" t="s">
-        <v>152</v>
-      </c>
       <c r="E42" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="F42" t="s">
         <v>185</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" t="s">
+        <v>184</v>
+      </c>
+      <c r="H42" s="2">
         <v>2.84</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>6</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="4">
         <f t="shared" si="0"/>
         <v>17.04</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G45" s="2" t="s">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I45" s="2">
-        <f>SUM(I4:I42)</f>
+      <c r="J45" s="4">
+        <f>SUM(J4:J42)</f>
         <v>97.380000000000024</v>
       </c>
     </row>

</xml_diff>